<commit_message>
Updated excel with KPI
</commit_message>
<xml_diff>
--- a/DB_schema_broker_retailer --(AutoRecovered).xlsx
+++ b/DB_schema_broker_retailer --(AutoRecovered).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pragalya Kanakaraj\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA412050-4485-4923-8EA3-ACC34222C43A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D408F36E-70E8-47C0-BD4B-9A523808B488}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{893E6BC4-BA8D-4CB6-8A87-F5D96D0468C5}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="911" uniqueCount="418">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="950" uniqueCount="444">
   <si>
     <t xml:space="preserve"> bid</t>
   </si>
@@ -735,9 +735,6 @@
     <t>stock_sold</t>
   </si>
   <si>
-    <t xml:space="preserve"> warehouse_id</t>
-  </si>
-  <si>
     <t>expiry_date</t>
   </si>
   <si>
@@ -1418,6 +1415,87 @@
   </si>
   <si>
     <t xml:space="preserve">sum(quantity - unit wrt product_id) </t>
+  </si>
+  <si>
+    <t>we could categarise based on filter like monthly , weekly , yearly</t>
+  </si>
+  <si>
+    <t>Seasonal Demand Patterns</t>
+  </si>
+  <si>
+    <t>delivery_date</t>
+  </si>
+  <si>
+    <t>1. Monthly Demand (in units)</t>
+  </si>
+  <si>
+    <t>SUM(quantity*unit_id)</t>
+  </si>
+  <si>
+    <t>Stock Levels</t>
+  </si>
+  <si>
+    <t>mandi_id --&gt; stock_table</t>
+  </si>
+  <si>
+    <t>stock_left --&gt; stock_table</t>
+  </si>
+  <si>
+    <t>product_id --&gt; master_product</t>
+  </si>
+  <si>
+    <t>updatedat --&gt; updatedAt</t>
+  </si>
+  <si>
+    <t>1.Current Stock per Product</t>
+  </si>
+  <si>
+    <t>SUM(stock_left) wrt product_id wrt mandi_id</t>
+  </si>
+  <si>
+    <t>2.Least Stocked Product</t>
+  </si>
+  <si>
+    <t>ORDER BY stock_left DESC / ASC</t>
+  </si>
+  <si>
+    <t>minimum_stock_level --&gt; stock_table</t>
+  </si>
+  <si>
+    <t>To flag low stock items</t>
+  </si>
+  <si>
+    <t>Maximum capacity of stock per product held in mandi</t>
+  </si>
+  <si>
+    <t>(stock_left / maximum_stock_level) * 100</t>
+  </si>
+  <si>
+    <t>to have a look on stock movement in certain mandi</t>
+  </si>
+  <si>
+    <t>unit_id --&gt; stock_id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">unit_id </t>
+  </si>
+  <si>
+    <t>Low Stock Items</t>
+  </si>
+  <si>
+    <t>stock_left</t>
+  </si>
+  <si>
+    <t>from stock table</t>
+  </si>
+  <si>
+    <t>1.Total Low Stock Items</t>
+  </si>
+  <si>
+    <t>if stock_left &lt; minimum_stock_level product_id wrt mandi_id</t>
+  </si>
+  <si>
+    <t>3.Stock availablity %</t>
   </si>
 </sst>
 </file>
@@ -1624,7 +1702,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -1662,6 +1740,9 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2052,13 +2133,13 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" s="8" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B12" s="9"/>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>23</v>
@@ -2066,7 +2147,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" s="4" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B14" s="5" t="s">
         <v>21</v>
@@ -2074,12 +2155,12 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B19" t="s">
         <v>23</v>
@@ -2095,7 +2176,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A21" s="2" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B21" s="3" t="s">
         <v>17</v>
@@ -2175,7 +2256,7 @@
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A31" s="2" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B31" s="3" t="s">
         <v>23</v>
@@ -2383,13 +2464,13 @@
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A72" s="8" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B72" s="9"/>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A73" s="2" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B73" s="3" t="s">
         <v>23</v>
@@ -2397,7 +2478,7 @@
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A74" s="2" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B74" t="s">
         <v>23</v>
@@ -2405,7 +2486,7 @@
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A75" s="2" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B75" s="3" t="s">
         <v>23</v>
@@ -2414,7 +2495,7 @@
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A76" s="4" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B76" s="5" t="s">
         <v>83</v>
@@ -2452,7 +2533,7 @@
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A83" s="2" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B83" s="3" t="s">
         <v>60</v>
@@ -2500,13 +2581,13 @@
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A91" s="8" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B91" s="9"/>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A92" s="2" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B92" s="3" t="s">
         <v>23</v>
@@ -2514,7 +2595,7 @@
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A93" s="2" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B93" s="3" t="s">
         <v>39</v>
@@ -2522,23 +2603,23 @@
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A94" s="2" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B94" s="3" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A95" s="2" t="s">
+        <v>255</v>
+      </c>
+      <c r="B95" s="3" t="s">
         <v>256</v>
-      </c>
-      <c r="B95" s="3" t="s">
-        <v>257</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A96" s="2" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B96" s="3" t="s">
         <v>39</v>
@@ -2546,39 +2627,39 @@
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A97" s="2" t="s">
+        <v>259</v>
+      </c>
+      <c r="B97" s="3" t="s">
         <v>260</v>
-      </c>
-      <c r="B97" s="3" t="s">
-        <v>261</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A98" s="2" t="s">
+        <v>261</v>
+      </c>
+      <c r="B98" s="3" t="s">
         <v>262</v>
-      </c>
-      <c r="B98" s="3" t="s">
-        <v>263</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A99" s="2" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="B99" s="3" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A100" s="4" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B100" s="5" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A104" s="8" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B104" s="9"/>
     </row>
@@ -2592,15 +2673,15 @@
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A106" s="2" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="B106" s="3" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A107" s="4" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B107" s="5" t="s">
         <v>18</v>
@@ -2622,10 +2703,10 @@
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A113" s="2" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="B113" s="3" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.35">
@@ -2633,7 +2714,7 @@
         <v>67</v>
       </c>
       <c r="B114" s="3" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.35">
@@ -2652,10 +2733,10 @@
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A120" s="2" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B120" s="3" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.35">
@@ -2668,7 +2749,7 @@
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A122" s="4" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="B122" s="5" t="s">
         <v>18</v>
@@ -2690,7 +2771,7 @@
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A128" s="2" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="B128" s="3" t="s">
         <v>18</v>
@@ -2808,13 +2889,13 @@
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A148" s="8" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B148" s="9"/>
     </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A149" s="2" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B149" s="3" t="s">
         <v>23</v>
@@ -2822,7 +2903,7 @@
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A150" s="2" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B150" s="3" t="s">
         <v>23</v>
@@ -2838,7 +2919,7 @@
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A152" s="4" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B152" s="5" t="s">
         <v>83</v>
@@ -3335,7 +3416,7 @@
     </row>
     <row r="252" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A252" s="8" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B252" s="9"/>
     </row>
@@ -3349,7 +3430,7 @@
     </row>
     <row r="254" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A254" s="4" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="B254" s="5" t="s">
         <v>38</v>
@@ -3366,10 +3447,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6C4FB58-CE7A-45E2-9E7C-C91A86D7AE77}">
-  <dimension ref="A1:L99"/>
+  <dimension ref="A1:L139"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A95" zoomScale="84" workbookViewId="0">
-      <selection activeCell="F90" sqref="F90"/>
+    <sheetView tabSelected="1" topLeftCell="A128" zoomScale="84" workbookViewId="0">
+      <selection activeCell="A142" sqref="A142"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3382,61 +3463,61 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
+        <v>328</v>
+      </c>
+      <c r="B2" t="s">
         <v>329</v>
-      </c>
-      <c r="B2" t="s">
-        <v>330</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B3" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B4" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B5" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
+        <v>333</v>
+      </c>
+      <c r="B7" t="s">
         <v>334</v>
-      </c>
-      <c r="B7" t="s">
-        <v>335</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
+        <v>338</v>
+      </c>
+      <c r="B19" t="s">
         <v>339</v>
-      </c>
-      <c r="B19" t="s">
-        <v>340</v>
       </c>
       <c r="F19" s="18"/>
       <c r="G19" s="19"/>
@@ -3446,16 +3527,16 @@
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B20" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="F20" s="20" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="J20" s="3"/>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.35">
       <c r="F21" s="2" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="J21" s="3"/>
     </row>
@@ -3464,7 +3545,7 @@
         <v>146</v>
       </c>
       <c r="G22" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="J22" s="3"/>
     </row>
@@ -3473,13 +3554,13 @@
         <v>69</v>
       </c>
       <c r="G23" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="J23" s="3"/>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.35">
       <c r="F24" s="4" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="G24" s="21"/>
       <c r="H24" s="21"/>
@@ -3488,7 +3569,7 @@
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.35">
       <c r="F27" s="8" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="G27" s="19"/>
       <c r="H27" s="19"/>
@@ -3508,7 +3589,7 @@
         <v>69</v>
       </c>
       <c r="G29" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="L29" s="3"/>
     </row>
@@ -3517,16 +3598,16 @@
         <v>145</v>
       </c>
       <c r="G30" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="L30" s="3"/>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.35">
       <c r="F31" s="2" t="s">
+        <v>353</v>
+      </c>
+      <c r="G31" t="s">
         <v>354</v>
-      </c>
-      <c r="G31" t="s">
-        <v>355</v>
       </c>
       <c r="L31" s="3"/>
     </row>
@@ -3535,7 +3616,7 @@
         <v>162</v>
       </c>
       <c r="G32" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="L32" s="3"/>
     </row>
@@ -3544,28 +3625,28 @@
         <v>79</v>
       </c>
       <c r="G33" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="L33" s="3"/>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.35">
       <c r="F34" s="2" t="s">
+        <v>349</v>
+      </c>
+      <c r="G34" t="s">
         <v>350</v>
-      </c>
-      <c r="G34" t="s">
-        <v>351</v>
       </c>
       <c r="L34" s="3"/>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.35">
       <c r="F35" s="2" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="L35" s="3"/>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.35">
       <c r="F36" s="4" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="G36" s="21"/>
       <c r="H36" s="21"/>
@@ -3576,13 +3657,13 @@
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
+        <v>357</v>
+      </c>
+      <c r="B40" t="s">
         <v>358</v>
       </c>
-      <c r="B40" t="s">
+      <c r="F40" s="8" t="s">
         <v>359</v>
-      </c>
-      <c r="F40" s="8" t="s">
-        <v>360</v>
       </c>
       <c r="G40" s="19"/>
       <c r="H40" s="19"/>
@@ -3590,31 +3671,31 @@
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B41" t="s">
+        <v>359</v>
+      </c>
+      <c r="F41" s="2" t="s">
         <v>360</v>
-      </c>
-      <c r="F41" s="2" t="s">
-        <v>361</v>
       </c>
       <c r="I41" s="3"/>
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B42" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="F42" s="2" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="G42" s="22" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="I42" s="3"/>
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.35">
       <c r="F43" s="2" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="G43" s="22" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="I43" s="3"/>
     </row>
@@ -3634,7 +3715,7 @@
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.35">
       <c r="F49" s="8" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="G49" s="19"/>
       <c r="H49" s="19"/>
@@ -3642,7 +3723,7 @@
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.35">
       <c r="F50" s="2" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="I50" s="3"/>
     </row>
@@ -3654,34 +3735,34 @@
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.35">
       <c r="F52" s="2" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="G52" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="I52" s="3"/>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.35">
       <c r="F53" s="2" t="s">
+        <v>368</v>
+      </c>
+      <c r="G53" t="s">
         <v>369</v>
-      </c>
-      <c r="G53" t="s">
-        <v>370</v>
       </c>
       <c r="I53" s="3"/>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.35">
       <c r="F54" s="2" t="s">
+        <v>370</v>
+      </c>
+      <c r="G54" t="s">
         <v>371</v>
-      </c>
-      <c r="G54" t="s">
-        <v>372</v>
       </c>
       <c r="I54" s="3"/>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.35">
       <c r="F55" s="4" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="G55" s="21"/>
       <c r="H55" s="21"/>
@@ -3689,7 +3770,7 @@
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A63" s="8" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="B63" s="19"/>
       <c r="C63" s="9"/>
@@ -3704,16 +3785,18 @@
     <row r="65" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A65" s="2"/>
       <c r="B65" s="25" t="s">
-        <v>385</v>
-      </c>
-      <c r="C65" s="3"/>
+        <v>384</v>
+      </c>
+      <c r="C65" s="3" t="s">
+        <v>417</v>
+      </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A66" s="2" t="s">
         <v>173</v>
       </c>
       <c r="B66" s="25" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="C66" s="3"/>
     </row>
@@ -3726,10 +3809,10 @@
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A68" s="2" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="B68" s="25" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="C68" s="3"/>
     </row>
@@ -3762,46 +3845,46 @@
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A74" s="20" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="B74" s="25"/>
       <c r="C74" s="3"/>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A75" s="2" t="s">
+        <v>390</v>
+      </c>
+      <c r="B75" s="25" t="s">
         <v>391</v>
       </c>
-      <c r="B75" s="25" t="s">
-        <v>392</v>
-      </c>
       <c r="C75" s="3" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A76" s="2" t="s">
+        <v>392</v>
+      </c>
+      <c r="B76" s="25" t="s">
         <v>393</v>
-      </c>
-      <c r="B76" s="25" t="s">
-        <v>394</v>
       </c>
       <c r="C76" s="3"/>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A77" s="2" t="s">
+        <v>395</v>
+      </c>
+      <c r="B77" s="25" t="s">
         <v>396</v>
-      </c>
-      <c r="B77" s="25" t="s">
-        <v>397</v>
       </c>
       <c r="C77" s="3"/>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A78" s="2" t="s">
+        <v>397</v>
+      </c>
+      <c r="B78" s="25" t="s">
         <v>398</v>
-      </c>
-      <c r="B78" s="25" t="s">
-        <v>399</v>
       </c>
       <c r="C78" s="3"/>
     </row>
@@ -3812,7 +3895,7 @@
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A83" s="8" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="B83" s="19"/>
       <c r="C83" s="9"/>
@@ -3827,14 +3910,14 @@
     <row r="85" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A85" s="2"/>
       <c r="B85" s="25" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="C85" s="3"/>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A86" s="2"/>
       <c r="B86" s="25" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="C86" s="3"/>
     </row>
@@ -3848,31 +3931,31 @@
     <row r="88" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A88" s="2"/>
       <c r="B88" s="25" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="C88" s="3"/>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A89" s="2"/>
       <c r="B89" s="25" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="C89" s="3"/>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A90" s="2"/>
       <c r="B90" s="26" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="C90" s="3"/>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A91" s="2"/>
       <c r="B91" s="25" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="C91" s="3" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.35">
@@ -3887,7 +3970,7 @@
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A94" s="20" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="B94" s="25"/>
       <c r="C94" s="3"/>
@@ -3899,43 +3982,290 @@
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A96" s="2" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="B96" s="25" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="C96" s="3" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A97" s="2" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="B97" s="25" t="s">
+        <v>409</v>
+      </c>
+      <c r="C97" s="3" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A98" s="27" t="s">
         <v>410</v>
       </c>
-      <c r="C97" s="3" t="s">
-        <v>417</v>
-      </c>
-    </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A98" s="2" t="s">
+      <c r="B98" s="26" t="s">
         <v>411</v>
       </c>
-      <c r="B98" s="25" t="s">
-        <v>412</v>
-      </c>
-      <c r="C98" s="3"/>
+      <c r="C98" s="28"/>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A99" s="4" t="s">
+        <v>413</v>
+      </c>
+      <c r="B99" s="21" t="s">
         <v>414</v>
       </c>
-      <c r="B99" s="21" t="s">
-        <v>415</v>
-      </c>
       <c r="C99" s="5"/>
+    </row>
+    <row r="102" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A102" s="8" t="s">
+        <v>418</v>
+      </c>
+      <c r="B102" s="9"/>
+    </row>
+    <row r="103" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A103" s="2"/>
+      <c r="B103" s="3" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A104" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="B104" s="3" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A105" s="2"/>
+      <c r="B105" s="3" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A106" s="2"/>
+      <c r="B106" s="3" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A107" s="2"/>
+      <c r="B107" s="3"/>
+    </row>
+    <row r="108" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A108" s="2"/>
+      <c r="B108" s="3"/>
+    </row>
+    <row r="109" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A109" s="20" t="s">
+        <v>389</v>
+      </c>
+      <c r="B109" s="3"/>
+    </row>
+    <row r="110" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A110" s="4" t="s">
+        <v>420</v>
+      </c>
+      <c r="B110" s="5" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="114" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A114" s="8" t="s">
+        <v>422</v>
+      </c>
+      <c r="B114" s="19"/>
+      <c r="C114" s="19"/>
+      <c r="D114" s="19"/>
+      <c r="E114" s="9"/>
+    </row>
+    <row r="115" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A115" s="2"/>
+      <c r="B115" s="25" t="s">
+        <v>425</v>
+      </c>
+      <c r="C115" s="25"/>
+      <c r="D115" s="25"/>
+      <c r="E115" s="3"/>
+    </row>
+    <row r="116" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A116" s="2"/>
+      <c r="B116" s="25" t="s">
+        <v>423</v>
+      </c>
+      <c r="C116" s="25"/>
+      <c r="D116" s="25"/>
+      <c r="E116" s="3"/>
+    </row>
+    <row r="117" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A117" s="2"/>
+      <c r="B117" s="25" t="s">
+        <v>424</v>
+      </c>
+      <c r="C117" s="25"/>
+      <c r="D117" s="25"/>
+      <c r="E117" s="3"/>
+    </row>
+    <row r="118" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A118" s="2"/>
+      <c r="B118" s="29" t="s">
+        <v>436</v>
+      </c>
+      <c r="C118" s="25"/>
+      <c r="D118" s="25"/>
+      <c r="E118" s="3"/>
+    </row>
+    <row r="119" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A119" s="2"/>
+      <c r="B119" s="25" t="s">
+        <v>426</v>
+      </c>
+      <c r="C119" s="25"/>
+      <c r="D119" s="25"/>
+      <c r="E119" s="3"/>
+    </row>
+    <row r="120" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A120" s="2"/>
+      <c r="B120" s="25" t="s">
+        <v>431</v>
+      </c>
+      <c r="C120" s="25" t="s">
+        <v>432</v>
+      </c>
+      <c r="D120" s="25"/>
+      <c r="E120" s="3"/>
+    </row>
+    <row r="121" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A121" s="2"/>
+      <c r="B121" s="25" t="s">
+        <v>199</v>
+      </c>
+      <c r="C121" s="25" t="s">
+        <v>433</v>
+      </c>
+      <c r="D121" s="25"/>
+      <c r="E121" s="3"/>
+    </row>
+    <row r="122" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A122" s="2"/>
+      <c r="D122" s="25"/>
+      <c r="E122" s="3"/>
+    </row>
+    <row r="123" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A123" s="20" t="s">
+        <v>389</v>
+      </c>
+      <c r="B123" s="25"/>
+      <c r="C123" s="25"/>
+      <c r="D123" s="25"/>
+      <c r="E123" s="3"/>
+    </row>
+    <row r="124" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A124" s="2" t="s">
+        <v>427</v>
+      </c>
+      <c r="B124" s="25" t="s">
+        <v>428</v>
+      </c>
+      <c r="C124" s="25"/>
+      <c r="D124" s="25"/>
+      <c r="E124" s="3"/>
+    </row>
+    <row r="125" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A125" s="2" t="s">
+        <v>429</v>
+      </c>
+      <c r="B125" s="25" t="s">
+        <v>430</v>
+      </c>
+      <c r="C125" s="25"/>
+      <c r="D125" s="25"/>
+      <c r="E125" s="3"/>
+    </row>
+    <row r="126" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A126" s="4" t="s">
+        <v>443</v>
+      </c>
+      <c r="B126" s="21" t="s">
+        <v>434</v>
+      </c>
+      <c r="C126" s="21" t="s">
+        <v>435</v>
+      </c>
+      <c r="D126" s="21"/>
+      <c r="E126" s="5"/>
+    </row>
+    <row r="130" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A130" s="8" t="s">
+        <v>438</v>
+      </c>
+      <c r="B130" s="19"/>
+      <c r="C130" s="9"/>
+    </row>
+    <row r="131" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A131" s="2"/>
+      <c r="B131" s="25"/>
+      <c r="C131" s="3"/>
+    </row>
+    <row r="132" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A132" s="2"/>
+      <c r="B132" s="25" t="s">
+        <v>79</v>
+      </c>
+      <c r="C132" s="3"/>
+    </row>
+    <row r="133" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A133" s="2" t="s">
+        <v>440</v>
+      </c>
+      <c r="B133" s="25" t="s">
+        <v>439</v>
+      </c>
+      <c r="C133" s="3"/>
+    </row>
+    <row r="134" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A134" s="2"/>
+      <c r="B134" s="25" t="s">
+        <v>198</v>
+      </c>
+      <c r="C134" s="3"/>
+    </row>
+    <row r="135" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A135" s="2"/>
+      <c r="B135" s="25" t="s">
+        <v>69</v>
+      </c>
+      <c r="C135" s="3"/>
+    </row>
+    <row r="136" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A136" s="2"/>
+      <c r="B136" s="25"/>
+      <c r="C136" s="3"/>
+    </row>
+    <row r="137" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A137" s="2"/>
+      <c r="B137" s="25"/>
+      <c r="C137" s="3"/>
+    </row>
+    <row r="138" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A138" s="20" t="s">
+        <v>389</v>
+      </c>
+      <c r="B138" s="25"/>
+      <c r="C138" s="3"/>
+    </row>
+    <row r="139" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A139" s="4" t="s">
+        <v>441</v>
+      </c>
+      <c r="B139" s="21" t="s">
+        <v>442</v>
+      </c>
+      <c r="C139" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3959,79 +4289,79 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
+        <v>296</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>297</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>298</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>299</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B3" t="s">
         <v>187</v>
       </c>
       <c r="C3" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="B5" t="s">
         <v>187</v>
       </c>
       <c r="C5" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="B7" t="s">
         <v>173</v>
       </c>
       <c r="C7" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
+        <v>303</v>
+      </c>
+      <c r="B9" t="s">
+        <v>214</v>
+      </c>
+      <c r="C9" t="s">
         <v>304</v>
-      </c>
-      <c r="B9" t="s">
-        <v>215</v>
-      </c>
-      <c r="C9" t="s">
-        <v>305</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="B11" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C11" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B14" t="s">
         <v>113</v>
       </c>
       <c r="C14" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
   </sheetData>
@@ -4041,10 +4371,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB499724-65CB-4F13-8120-13A79F1C18BE}">
-  <dimension ref="A1:K187"/>
+  <dimension ref="A1:K189"/>
   <sheetViews>
-    <sheetView topLeftCell="A174" zoomScale="94" workbookViewId="0">
-      <selection activeCell="C165" sqref="C165"/>
+    <sheetView topLeftCell="A94" zoomScale="94" workbookViewId="0">
+      <selection activeCell="E101" sqref="E101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4145,7 +4475,7 @@
         <v>136</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.35">
@@ -4666,7 +4996,7 @@
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A98" s="2" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B98" s="3" t="s">
         <v>23</v>
@@ -4705,16 +5035,12 @@
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A103" s="2" t="s">
-        <v>174</v>
-      </c>
-      <c r="B103" s="3" t="s">
-        <v>62</v>
-      </c>
+      <c r="A103" s="2"/>
+      <c r="B103" s="3"/>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A104" s="2" t="s">
-        <v>196</v>
+        <v>437</v>
       </c>
       <c r="B104" s="3" t="s">
         <v>23</v>
@@ -4722,7 +5048,7 @@
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A105" s="2" t="s">
-        <v>197</v>
+        <v>174</v>
       </c>
       <c r="B105" s="3" t="s">
         <v>62</v>
@@ -4730,77 +5056,77 @@
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A106" s="2" t="s">
-        <v>198</v>
+        <v>69</v>
       </c>
       <c r="B106" s="3" t="s">
-        <v>62</v>
+        <v>23</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A107" s="2" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="B107" s="3" t="s">
-        <v>100</v>
+        <v>62</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A108" s="2" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="B108" s="3" t="s">
-        <v>100</v>
+        <v>62</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A109" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="B109" s="3" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A110" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="B110" s="3" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A111" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="B111" s="3" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A112" s="4" t="s">
         <v>201</v>
       </c>
-      <c r="B109" s="3" t="s">
+      <c r="B112" s="5" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A110" s="4" t="s">
+    <row r="116" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A116" s="8" t="s">
         <v>202</v>
       </c>
-      <c r="B110" s="5" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="114" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A114" s="8" t="s">
-        <v>203</v>
-      </c>
-      <c r="B114" s="9"/>
-    </row>
-    <row r="115" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A115" s="2" t="s">
-        <v>204</v>
-      </c>
-      <c r="B115" s="3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="116" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A116" s="2" t="s">
-        <v>205</v>
-      </c>
-      <c r="B116" s="3" t="s">
-        <v>210</v>
-      </c>
+      <c r="B116" s="9"/>
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A117" s="2" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="B117" s="3" t="s">
-        <v>210</v>
+        <v>23</v>
       </c>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A118" s="2" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="B118" s="3" t="s">
         <v>209</v>
@@ -4808,235 +5134,235 @@
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A119" s="2" t="s">
-        <v>117</v>
+        <v>205</v>
       </c>
       <c r="B119" s="3" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A120" s="2" t="s">
-        <v>179</v>
+        <v>206</v>
       </c>
       <c r="B120" s="3" t="s">
-        <v>23</v>
+        <v>208</v>
       </c>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A121" s="2" t="s">
-        <v>180</v>
+        <v>117</v>
       </c>
       <c r="B121" s="3" t="s">
-        <v>23</v>
+        <v>210</v>
       </c>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A122" s="2" t="s">
-        <v>118</v>
+        <v>179</v>
       </c>
       <c r="B122" s="3" t="s">
-        <v>183</v>
+        <v>23</v>
       </c>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A123" s="2" t="s">
-        <v>208</v>
+        <v>180</v>
       </c>
       <c r="B123" s="3" t="s">
-        <v>184</v>
+        <v>23</v>
       </c>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A124" s="2" t="s">
-        <v>36</v>
+        <v>118</v>
       </c>
       <c r="B124" s="3" t="s">
-        <v>119</v>
+        <v>183</v>
       </c>
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A125" s="2" t="s">
+        <v>207</v>
+      </c>
+      <c r="B125" s="3" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="126" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A126" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B126" s="3" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="127" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A127" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="B125" s="3" t="s">
+      <c r="B127" s="3" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="126" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A126" s="4" t="s">
+    <row r="128" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A128" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="B126" s="5" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="130" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A130" s="8" t="s">
-        <v>270</v>
-      </c>
-      <c r="B130" s="9"/>
-    </row>
-    <row r="131" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A131" s="2" t="s">
-        <v>271</v>
-      </c>
-      <c r="B131" s="3" t="s">
-        <v>278</v>
+      <c r="B128" s="5" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A132" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="B132" s="3" t="s">
-        <v>23</v>
-      </c>
+      <c r="A132" s="8" t="s">
+        <v>269</v>
+      </c>
+      <c r="B132" s="9"/>
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A133" s="2" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="B133" s="3" t="s">
-        <v>62</v>
+        <v>277</v>
       </c>
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A134" s="2" t="s">
-        <v>273</v>
+        <v>127</v>
       </c>
       <c r="B134" s="3" t="s">
-        <v>279</v>
+        <v>23</v>
       </c>
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A135" s="2" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="B135" s="3" t="s">
-        <v>18</v>
+        <v>62</v>
       </c>
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A136" s="2" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="B136" s="3" t="s">
-        <v>23</v>
+        <v>278</v>
       </c>
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A137" s="2" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="B137" s="3" t="s">
-        <v>279</v>
+        <v>18</v>
       </c>
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A138" s="2" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="B138" s="3" t="s">
-        <v>62</v>
+        <v>23</v>
       </c>
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A139" s="2" t="s">
+        <v>275</v>
+      </c>
+      <c r="B139" s="3" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="140" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A140" s="2" t="s">
+        <v>276</v>
+      </c>
+      <c r="B140" s="3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="141" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A141" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B139" s="3" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="140" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A140" s="4" t="s">
+      <c r="B141" s="3" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="142" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A142" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="B140" s="5" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="144" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A144" s="8" t="s">
+      <c r="B142" s="5" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="146" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A146" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="B146" s="9"/>
+    </row>
+    <row r="147" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A147" s="2" t="s">
         <v>280</v>
       </c>
-      <c r="B144" s="9"/>
-    </row>
-    <row r="145" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A145" s="2" t="s">
+      <c r="B147" s="3" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="148" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A148" s="4" t="s">
         <v>281</v>
       </c>
-      <c r="B145" s="3" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="146" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A146" s="4" t="s">
-        <v>282</v>
-      </c>
-      <c r="B146" s="5" t="s">
+      <c r="B148" s="5" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="150" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A150" s="8" t="s">
-        <v>311</v>
-      </c>
-      <c r="B150" s="9"/>
-      <c r="C150" s="19"/>
-      <c r="D150" s="19"/>
-      <c r="E150" s="19"/>
-      <c r="F150" s="19"/>
-      <c r="G150" s="19"/>
-      <c r="H150" s="19"/>
-      <c r="I150" s="19"/>
-      <c r="J150" s="19"/>
-      <c r="K150" s="9"/>
-    </row>
-    <row r="151" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A151" s="2" t="s">
-        <v>178</v>
-      </c>
-      <c r="B151" s="3"/>
-      <c r="K151" s="3"/>
-    </row>
     <row r="152" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A152" s="2" t="s">
-        <v>312</v>
-      </c>
-      <c r="B152" s="3" t="s">
-        <v>152</v>
-      </c>
-      <c r="K152" s="3"/>
+      <c r="A152" s="8" t="s">
+        <v>310</v>
+      </c>
+      <c r="B152" s="9"/>
+      <c r="C152" s="19"/>
+      <c r="D152" s="19"/>
+      <c r="E152" s="19"/>
+      <c r="F152" s="19"/>
+      <c r="G152" s="19"/>
+      <c r="H152" s="19"/>
+      <c r="I152" s="19"/>
+      <c r="J152" s="19"/>
+      <c r="K152" s="9"/>
     </row>
     <row r="153" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A153" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="B153" s="3"/>
+      <c r="K153" s="3"/>
+    </row>
+    <row r="154" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A154" s="2" t="s">
+        <v>311</v>
+      </c>
+      <c r="B154" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="K154" s="3"/>
+    </row>
+    <row r="155" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A155" s="2" t="s">
+        <v>373</v>
+      </c>
+      <c r="B155" s="3" t="s">
         <v>374</v>
       </c>
-      <c r="B153" s="3" t="s">
+      <c r="C155" t="s">
+        <v>79</v>
+      </c>
+      <c r="D155" t="s">
         <v>375</v>
-      </c>
-      <c r="C153" t="s">
-        <v>79</v>
-      </c>
-      <c r="D153" t="s">
-        <v>376</v>
-      </c>
-      <c r="K153" s="3"/>
-    </row>
-    <row r="154" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A154" s="2"/>
-      <c r="B154" s="3"/>
-      <c r="C154" t="s">
-        <v>155</v>
-      </c>
-      <c r="K154" s="3"/>
-    </row>
-    <row r="155" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A155" s="2"/>
-      <c r="B155" s="3"/>
-      <c r="C155" t="s">
-        <v>145</v>
       </c>
       <c r="K155" s="3"/>
     </row>
@@ -5044,203 +5370,219 @@
       <c r="A156" s="2"/>
       <c r="B156" s="3"/>
       <c r="C156" t="s">
-        <v>381</v>
-      </c>
-      <c r="D156" t="s">
-        <v>382</v>
+        <v>155</v>
       </c>
       <c r="K156" s="3"/>
     </row>
     <row r="157" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A157" s="2"/>
       <c r="B157" s="3"/>
+      <c r="C157" t="s">
+        <v>145</v>
+      </c>
       <c r="K157" s="3"/>
     </row>
     <row r="158" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A158" s="2"/>
       <c r="B158" s="3"/>
       <c r="C158" t="s">
-        <v>377</v>
+        <v>380</v>
       </c>
       <c r="D158" t="s">
-        <v>378</v>
+        <v>381</v>
       </c>
       <c r="K158" s="3"/>
     </row>
     <row r="159" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A159" s="2"/>
       <c r="B159" s="3"/>
-      <c r="C159" t="s">
-        <v>379</v>
-      </c>
-      <c r="D159" t="s">
-        <v>380</v>
-      </c>
       <c r="K159" s="3"/>
     </row>
     <row r="160" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A160" s="2"/>
       <c r="B160" s="3"/>
       <c r="C160" t="s">
-        <v>146</v>
+        <v>376</v>
+      </c>
+      <c r="D160" t="s">
+        <v>377</v>
       </c>
       <c r="K160" s="3"/>
     </row>
     <row r="161" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A161" s="2"/>
       <c r="B161" s="3"/>
-      <c r="C161" s="4" t="s">
-        <v>383</v>
-      </c>
-      <c r="D161" s="21" t="s">
-        <v>263</v>
-      </c>
-      <c r="E161" s="21"/>
-      <c r="F161" s="21"/>
-      <c r="G161" s="21"/>
-      <c r="H161" s="21"/>
-      <c r="I161" s="21"/>
-      <c r="J161" s="21"/>
-      <c r="K161" s="5"/>
+      <c r="C161" t="s">
+        <v>378</v>
+      </c>
+      <c r="D161" t="s">
+        <v>379</v>
+      </c>
+      <c r="K161" s="3"/>
+    </row>
+    <row r="162" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A162" s="2"/>
+      <c r="B162" s="3"/>
+      <c r="C162" t="s">
+        <v>146</v>
+      </c>
+      <c r="K162" s="3"/>
     </row>
     <row r="163" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A163" s="23"/>
-      <c r="B163" s="24"/>
-    </row>
-    <row r="171" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A171" s="14" t="s">
-        <v>315</v>
-      </c>
-      <c r="B171" s="15"/>
-    </row>
-    <row r="172" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A172" s="2" t="s">
-        <v>192</v>
-      </c>
-      <c r="B172" s="3" t="s">
-        <v>23</v>
-      </c>
+      <c r="A163" s="2"/>
+      <c r="B163" s="3"/>
+      <c r="C163" s="4" t="s">
+        <v>382</v>
+      </c>
+      <c r="D163" s="21" t="s">
+        <v>262</v>
+      </c>
+      <c r="E163" s="21"/>
+      <c r="F163" s="21"/>
+      <c r="G163" s="21"/>
+      <c r="H163" s="21"/>
+      <c r="I163" s="21"/>
+      <c r="J163" s="21"/>
+      <c r="K163" s="5"/>
+    </row>
+    <row r="165" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A165" s="23"/>
+      <c r="B165" s="24"/>
     </row>
     <row r="173" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A173" s="2" t="s">
-        <v>316</v>
-      </c>
-      <c r="B173" s="3" t="s">
-        <v>152</v>
-      </c>
+      <c r="A173" s="14" t="s">
+        <v>314</v>
+      </c>
+      <c r="B173" s="15"/>
     </row>
     <row r="174" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A174" s="2" t="s">
-        <v>178</v>
+        <v>192</v>
       </c>
       <c r="B174" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="C174" t="s">
-        <v>319</v>
+        <v>23</v>
       </c>
     </row>
     <row r="175" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A175" s="2" t="s">
-        <v>146</v>
+        <v>315</v>
       </c>
       <c r="B175" s="3" t="s">
-        <v>82</v>
+        <v>152</v>
       </c>
     </row>
     <row r="176" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A176" s="2" t="s">
-        <v>79</v>
+        <v>178</v>
       </c>
       <c r="B176" s="3" t="s">
         <v>82</v>
       </c>
+      <c r="C176" t="s">
+        <v>318</v>
+      </c>
     </row>
     <row r="177" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A177" s="2" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="B177" s="3" t="s">
-        <v>23</v>
+        <v>82</v>
       </c>
     </row>
     <row r="178" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A178" s="2" t="s">
-        <v>318</v>
+        <v>79</v>
       </c>
       <c r="B178" s="3" t="s">
-        <v>279</v>
+        <v>82</v>
       </c>
     </row>
     <row r="179" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A179" s="2" t="s">
-        <v>320</v>
+        <v>145</v>
       </c>
       <c r="B179" s="3" t="s">
-        <v>279</v>
+        <v>23</v>
       </c>
     </row>
     <row r="180" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A180" s="2" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="B180" s="3" t="s">
-        <v>325</v>
+        <v>278</v>
       </c>
     </row>
     <row r="181" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A181" s="2" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
       <c r="B181" s="3" t="s">
-        <v>18</v>
+        <v>278</v>
       </c>
     </row>
     <row r="182" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A182" s="2" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="B182" s="3" t="s">
         <v>324</v>
       </c>
     </row>
     <row r="183" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A183" s="17" t="s">
-        <v>326</v>
-      </c>
-      <c r="B183" s="16" t="s">
-        <v>327</v>
+      <c r="A183" s="2" t="s">
+        <v>321</v>
+      </c>
+      <c r="B183" s="3" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="184" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A184" s="2" t="s">
-        <v>155</v>
+        <v>322</v>
       </c>
       <c r="B184" s="3" t="s">
-        <v>279</v>
+        <v>323</v>
       </c>
     </row>
     <row r="185" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A185" s="2" t="s">
-        <v>317</v>
-      </c>
-      <c r="B185" s="3" t="s">
-        <v>314</v>
+      <c r="A185" s="17" t="s">
+        <v>325</v>
+      </c>
+      <c r="B185" s="16" t="s">
+        <v>326</v>
       </c>
     </row>
     <row r="186" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A186" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="B186" s="3" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="187" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A187" s="2" t="s">
+        <v>316</v>
+      </c>
+      <c r="B187" s="3" t="s">
         <v>313</v>
       </c>
-      <c r="B186" s="3" t="s">
+    </row>
+    <row r="188" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A188" s="2" t="s">
+        <v>312</v>
+      </c>
+      <c r="B188" s="3" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="187" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A187" s="4" t="s">
+    <row r="189" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A189" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="B187" s="5" t="s">
+      <c r="B189" s="5" t="s">
         <v>119</v>
       </c>
     </row>
@@ -5267,13 +5609,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>212</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>213</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>214</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
@@ -5283,37 +5625,37 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="B3" t="s">
         <v>215</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>216</v>
-      </c>
-      <c r="C3" t="s">
-        <v>217</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B4" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C4" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B5" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C5" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B6" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C6" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.35">
@@ -5321,34 +5663,34 @@
         <v>24</v>
       </c>
       <c r="B10" t="s">
+        <v>215</v>
+      </c>
+      <c r="C10" t="s">
         <v>216</v>
-      </c>
-      <c r="C10" t="s">
-        <v>217</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B11" t="s">
+        <v>217</v>
+      </c>
+      <c r="C11" t="s">
         <v>218</v>
-      </c>
-      <c r="C11" t="s">
-        <v>219</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B12" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C12" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B13" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C13" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.35">
@@ -5356,48 +5698,48 @@
         <v>27</v>
       </c>
       <c r="B17" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C17" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B18" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C18" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B19" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C19" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B20" t="s">
+        <v>220</v>
+      </c>
+      <c r="C20" t="s">
         <v>221</v>
-      </c>
-      <c r="C20" t="s">
-        <v>222</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.35">
@@ -5405,10 +5747,10 @@
         <v>42</v>
       </c>
       <c r="B25" t="s">
+        <v>215</v>
+      </c>
+      <c r="C25" t="s">
         <v>216</v>
-      </c>
-      <c r="C25" t="s">
-        <v>217</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.35">
@@ -5416,10 +5758,10 @@
         <v>102</v>
       </c>
       <c r="B26" t="s">
+        <v>217</v>
+      </c>
+      <c r="C26" t="s">
         <v>218</v>
-      </c>
-      <c r="C26" t="s">
-        <v>219</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.35">
@@ -5427,18 +5769,18 @@
         <v>110</v>
       </c>
       <c r="B27" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C27" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B28" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C28" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.35">
@@ -5446,34 +5788,34 @@
         <v>45</v>
       </c>
       <c r="B32" t="s">
+        <v>215</v>
+      </c>
+      <c r="C32" t="s">
         <v>216</v>
-      </c>
-      <c r="C32" t="s">
-        <v>217</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B33" t="s">
+        <v>217</v>
+      </c>
+      <c r="C33" t="s">
         <v>218</v>
-      </c>
-      <c r="C33" t="s">
-        <v>219</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B34" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C34" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B35" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C35" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.35">
@@ -5481,34 +5823,34 @@
         <v>51</v>
       </c>
       <c r="B39" t="s">
+        <v>215</v>
+      </c>
+      <c r="C39" t="s">
         <v>216</v>
-      </c>
-      <c r="C39" t="s">
-        <v>217</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B40" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C40" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B41" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C41" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B42" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C42" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.35">
@@ -5516,69 +5858,69 @@
         <v>65</v>
       </c>
       <c r="B46" t="s">
+        <v>215</v>
+      </c>
+      <c r="C46" t="s">
         <v>216</v>
-      </c>
-      <c r="C46" t="s">
-        <v>217</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B47" t="s">
+        <v>217</v>
+      </c>
+      <c r="C47" t="s">
         <v>218</v>
-      </c>
-      <c r="C47" t="s">
-        <v>219</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B48" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C48" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B49" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C49" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A53" s="1" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B53" t="s">
+        <v>215</v>
+      </c>
+      <c r="C53" t="s">
         <v>216</v>
-      </c>
-      <c r="C53" t="s">
-        <v>217</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B54" t="s">
+        <v>217</v>
+      </c>
+      <c r="C54" t="s">
         <v>218</v>
-      </c>
-      <c r="C54" t="s">
-        <v>219</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B55" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C55" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B56" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C56" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.35">
@@ -5586,43 +5928,43 @@
         <v>68</v>
       </c>
       <c r="B60" t="s">
+        <v>215</v>
+      </c>
+      <c r="C60" t="s">
         <v>216</v>
-      </c>
-      <c r="C60" t="s">
-        <v>217</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B61" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C61" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="B62" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C62" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B63" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C63" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.35">
@@ -5630,34 +5972,34 @@
         <v>78</v>
       </c>
       <c r="B67" t="s">
+        <v>215</v>
+      </c>
+      <c r="C67" t="s">
         <v>216</v>
-      </c>
-      <c r="C67" t="s">
-        <v>217</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B68" t="s">
+        <v>217</v>
+      </c>
+      <c r="C68" t="s">
         <v>218</v>
-      </c>
-      <c r="C68" t="s">
-        <v>219</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B69" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C69" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B70" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C70" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.35">
@@ -5665,34 +6007,34 @@
         <v>113</v>
       </c>
       <c r="B74" t="s">
+        <v>215</v>
+      </c>
+      <c r="C74" t="s">
         <v>216</v>
-      </c>
-      <c r="C74" t="s">
-        <v>217</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B75" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C75" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B76" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C76" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B77" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C77" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.35">
@@ -5700,48 +6042,48 @@
         <v>122</v>
       </c>
       <c r="B81" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C81" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B82" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C82" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B83" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C83" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B84" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C84" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.35">
@@ -5749,34 +6091,34 @@
         <v>143</v>
       </c>
       <c r="B89" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C89" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B90" t="s">
+        <v>217</v>
+      </c>
+      <c r="C90" t="s">
         <v>218</v>
-      </c>
-      <c r="C90" t="s">
-        <v>219</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B91" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C91" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B92" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C92" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.35">
@@ -5784,34 +6126,34 @@
         <v>151</v>
       </c>
       <c r="B96" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C96" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B97" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C97" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B98" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C98" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B99" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C99" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.35">
@@ -5819,34 +6161,34 @@
         <v>158</v>
       </c>
       <c r="B103" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C103" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B104" t="s">
+        <v>217</v>
+      </c>
+      <c r="C104" t="s">
         <v>218</v>
-      </c>
-      <c r="C104" t="s">
-        <v>219</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B105" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C105" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B106" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C106" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.35">
@@ -5854,34 +6196,34 @@
         <v>173</v>
       </c>
       <c r="B110" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C110" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B111" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C111" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B112" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C112" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B113" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C113" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.35">
@@ -5889,34 +6231,34 @@
         <v>187</v>
       </c>
       <c r="B117" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C117" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B118" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C118" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B119" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C119" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B120" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C120" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.35">
@@ -5924,10 +6266,10 @@
         <v>94</v>
       </c>
       <c r="B124" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C124" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.35">
@@ -5935,7 +6277,7 @@
         <v>92</v>
       </c>
       <c r="B125" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.35">
@@ -5943,7 +6285,7 @@
         <v>93</v>
       </c>
       <c r="B126" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.35">
@@ -5951,7 +6293,7 @@
         <v>85</v>
       </c>
       <c r="B127" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.35">
@@ -5959,34 +6301,34 @@
         <v>107</v>
       </c>
       <c r="B131" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C131" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B132" t="s">
+        <v>217</v>
+      </c>
+      <c r="C132" t="s">
         <v>218</v>
-      </c>
-      <c r="C132" t="s">
-        <v>219</v>
       </c>
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B133" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C133" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B134" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C134" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.35">
@@ -5994,12 +6336,12 @@
         <v>126</v>
       </c>
       <c r="B137" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B138" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated API for sales trend
</commit_message>
<xml_diff>
--- a/DB_schema_broker_retailer --(AutoRecovered).xlsx
+++ b/DB_schema_broker_retailer --(AutoRecovered).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\new_go_backend\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1E50E2D-B786-445F-87E5-43537127AC84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0747FFDF-5A4C-45AD-BB46-369CCBBE4189}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{893E6BC4-BA8D-4CB6-8A87-F5D96D0468C5}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="983" uniqueCount="466">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="985" uniqueCount="471">
   <si>
     <t xml:space="preserve"> bid</t>
   </si>
@@ -1318,12 +1318,6 @@
     <t>Sales Trends</t>
   </si>
   <si>
-    <t xml:space="preserve">delivery_date </t>
-  </si>
-  <si>
-    <t>price_of_each_order</t>
-  </si>
-  <si>
     <t>sum(price_of_each_order)</t>
   </si>
   <si>
@@ -1342,15 +1336,6 @@
     <t>Total revenue per month</t>
   </si>
   <si>
-    <t>2.Number of Orders</t>
-  </si>
-  <si>
-    <t>Total orders placed each month</t>
-  </si>
-  <si>
-    <t>b_branch_id --&gt;wrt the wholeseller_id</t>
-  </si>
-  <si>
     <t>3.Branch-wise Sales</t>
   </si>
   <si>
@@ -1562,6 +1547,36 @@
   </si>
   <si>
     <t>Helps wholesellers or retailers quickly identify where to buy each product.</t>
+  </si>
+  <si>
+    <t>club with cold storage - &gt; cost benefit analysis</t>
+  </si>
+  <si>
+    <t>inter-se stocks at mandi in geo loc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">indl wholeseller lvl </t>
+  </si>
+  <si>
+    <t xml:space="preserve">alert when high demand stocks are running out </t>
+  </si>
+  <si>
+    <t xml:space="preserve">actual_delivery_date </t>
+  </si>
+  <si>
+    <t xml:space="preserve">final_amount </t>
+  </si>
+  <si>
+    <t>business_schema.order_table</t>
+  </si>
+  <si>
+    <t>wholeseller_id --&gt; frm admin_schema.business_table(bid)</t>
+  </si>
+  <si>
+    <t>b_branch_id --&gt;wrt the wholeseller_id frm admin_schema.business_branch_table</t>
+  </si>
+  <si>
+    <t>retailer_id --&gt; --&gt; frm admin_schema.business_table(bid)</t>
   </si>
 </sst>
 </file>
@@ -1768,7 +1783,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -1807,7 +1822,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3514,8 +3528,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6C4FB58-CE7A-45E2-9E7C-C91A86D7AE77}">
   <dimension ref="A1:L174"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A127" zoomScale="84" workbookViewId="0">
-      <selection activeCell="F171" sqref="F171"/>
+    <sheetView tabSelected="1" topLeftCell="A62" zoomScale="103" workbookViewId="0">
+      <selection activeCell="A74" sqref="A74:C78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3842,49 +3856,48 @@
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A64" s="2"/>
-      <c r="B64" t="s">
-        <v>161</v>
-      </c>
       <c r="C64" s="3"/>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A65" s="2"/>
+      <c r="A65" s="2" t="s">
+        <v>467</v>
+      </c>
       <c r="B65" t="s">
-        <v>384</v>
+        <v>465</v>
       </c>
       <c r="C65" s="3" t="s">
-        <v>417</v>
+        <v>412</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A66" s="2" t="s">
-        <v>173</v>
+        <v>467</v>
       </c>
       <c r="B66" t="s">
-        <v>385</v>
+        <v>466</v>
       </c>
       <c r="C66" s="3"/>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A67" s="2"/>
       <c r="B67" t="s">
-        <v>146</v>
+        <v>468</v>
       </c>
       <c r="C67" s="3"/>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A68" s="2" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="B68" t="s">
-        <v>394</v>
+        <v>469</v>
       </c>
       <c r="C68" s="3"/>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A69" s="2"/>
       <c r="B69" t="s">
-        <v>178</v>
+        <v>470</v>
       </c>
       <c r="C69" s="3"/>
     </row>
@@ -3906,45 +3919,40 @@
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A74" s="20" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="C74" s="3"/>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A75" s="2" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="B75" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="C75" s="3" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A76" s="2" t="s">
-        <v>392</v>
-      </c>
-      <c r="B76" t="s">
-        <v>393</v>
-      </c>
+      <c r="A76" s="2"/>
       <c r="C76" s="3"/>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A77" s="2" t="s">
-        <v>395</v>
+        <v>390</v>
       </c>
       <c r="B77" t="s">
-        <v>396</v>
+        <v>391</v>
       </c>
       <c r="C77" s="3"/>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A78" s="2" t="s">
-        <v>397</v>
+        <v>392</v>
       </c>
       <c r="B78" t="s">
-        <v>398</v>
+        <v>393</v>
       </c>
       <c r="C78" s="3"/>
     </row>
@@ -3955,7 +3963,7 @@
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A83" s="8" t="s">
-        <v>403</v>
+        <v>398</v>
       </c>
       <c r="B83" s="19"/>
       <c r="C83" s="9"/>
@@ -3970,14 +3978,14 @@
     <row r="85" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A85" s="2"/>
       <c r="B85" t="s">
-        <v>399</v>
+        <v>394</v>
       </c>
       <c r="C85" s="3"/>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A86" s="2"/>
       <c r="B86" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="C86" s="3"/>
     </row>
@@ -3991,31 +3999,31 @@
     <row r="88" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A88" s="2"/>
       <c r="B88" t="s">
-        <v>400</v>
+        <v>395</v>
       </c>
       <c r="C88" s="3"/>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A89" s="2"/>
       <c r="B89" t="s">
-        <v>401</v>
+        <v>396</v>
       </c>
       <c r="C89" s="3"/>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A90" s="2"/>
       <c r="B90" s="25" t="s">
-        <v>402</v>
+        <v>397</v>
       </c>
       <c r="C90" s="3"/>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A91" s="2"/>
       <c r="B91" t="s">
-        <v>405</v>
+        <v>400</v>
       </c>
       <c r="C91" s="3" t="s">
-        <v>415</v>
+        <v>410</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.35">
@@ -4028,7 +4036,7 @@
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A94" s="20" t="s">
-        <v>404</v>
+        <v>399</v>
       </c>
       <c r="C94" s="3"/>
     </row>
@@ -4038,47 +4046,47 @@
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A96" s="2" t="s">
-        <v>406</v>
+        <v>401</v>
       </c>
       <c r="B96" t="s">
-        <v>408</v>
+        <v>403</v>
       </c>
       <c r="C96" s="3" t="s">
-        <v>412</v>
+        <v>407</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A97" s="2" t="s">
-        <v>407</v>
+        <v>402</v>
       </c>
       <c r="B97" t="s">
-        <v>409</v>
+        <v>404</v>
       </c>
       <c r="C97" s="3" t="s">
-        <v>416</v>
+        <v>411</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A98" s="26" t="s">
-        <v>410</v>
+        <v>405</v>
       </c>
       <c r="B98" s="25" t="s">
-        <v>411</v>
+        <v>406</v>
       </c>
       <c r="C98" s="27"/>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A99" s="4" t="s">
-        <v>413</v>
+        <v>408</v>
       </c>
       <c r="B99" s="21" t="s">
-        <v>414</v>
+        <v>409</v>
       </c>
       <c r="C99" s="5"/>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A102" s="8" t="s">
-        <v>418</v>
+        <v>413</v>
       </c>
       <c r="B102" s="9"/>
     </row>
@@ -4087,6 +4095,9 @@
       <c r="B103" s="3" t="s">
         <v>79</v>
       </c>
+      <c r="C103" t="s">
+        <v>461</v>
+      </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A104" s="2" t="s">
@@ -4105,7 +4116,7 @@
     <row r="106" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A106" s="2"/>
       <c r="B106" s="3" t="s">
-        <v>419</v>
+        <v>414</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.35">
@@ -4118,21 +4129,21 @@
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A109" s="20" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="B109" s="3"/>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A110" s="4" t="s">
-        <v>420</v>
+        <v>415</v>
       </c>
       <c r="B110" s="5" t="s">
-        <v>421</v>
+        <v>416</v>
       </c>
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A114" s="8" t="s">
-        <v>422</v>
+        <v>417</v>
       </c>
       <c r="B114" s="19"/>
       <c r="C114" s="19"/>
@@ -4142,45 +4153,48 @@
     <row r="115" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A115" s="2"/>
       <c r="B115" t="s">
-        <v>425</v>
+        <v>420</v>
       </c>
       <c r="E115" s="3"/>
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A116" s="2"/>
       <c r="B116" t="s">
-        <v>423</v>
+        <v>418</v>
+      </c>
+      <c r="C116" t="s">
+        <v>462</v>
       </c>
       <c r="E116" s="3"/>
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A117" s="2"/>
       <c r="B117" t="s">
-        <v>424</v>
+        <v>419</v>
       </c>
       <c r="E117" s="3"/>
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A118" s="2"/>
       <c r="B118" t="s">
-        <v>436</v>
+        <v>431</v>
       </c>
       <c r="E118" s="3"/>
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A119" s="2"/>
       <c r="B119" t="s">
-        <v>426</v>
+        <v>421</v>
       </c>
       <c r="E119" s="3"/>
     </row>
     <row r="120" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A120" s="2"/>
       <c r="B120" t="s">
-        <v>431</v>
+        <v>426</v>
       </c>
       <c r="C120" t="s">
-        <v>432</v>
+        <v>427</v>
       </c>
       <c r="E120" s="3"/>
     </row>
@@ -4190,7 +4204,7 @@
         <v>199</v>
       </c>
       <c r="C121" t="s">
-        <v>433</v>
+        <v>428</v>
       </c>
       <c r="E121" s="3"/>
     </row>
@@ -4200,65 +4214,69 @@
     </row>
     <row r="123" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A123" s="20" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="E123" s="3"/>
     </row>
     <row r="124" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A124" s="2" t="s">
-        <v>427</v>
+        <v>422</v>
       </c>
       <c r="B124" t="s">
-        <v>428</v>
+        <v>423</v>
       </c>
       <c r="E124" s="3"/>
     </row>
     <row r="125" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A125" s="2" t="s">
-        <v>429</v>
+        <v>424</v>
       </c>
       <c r="B125" t="s">
-        <v>430</v>
+        <v>425</v>
       </c>
       <c r="E125" s="3"/>
     </row>
     <row r="126" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A126" s="4" t="s">
-        <v>443</v>
+        <v>438</v>
       </c>
       <c r="B126" s="21" t="s">
-        <v>434</v>
+        <v>429</v>
       </c>
       <c r="C126" s="21" t="s">
-        <v>435</v>
+        <v>430</v>
       </c>
       <c r="D126" s="21"/>
       <c r="E126" s="5"/>
     </row>
     <row r="130" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A130" s="8" t="s">
-        <v>438</v>
+        <v>433</v>
       </c>
       <c r="B130" s="19"/>
       <c r="C130" s="9"/>
     </row>
     <row r="131" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A131" s="2"/>
-      <c r="C131" s="3"/>
+      <c r="C131" s="3" t="s">
+        <v>463</v>
+      </c>
     </row>
     <row r="132" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A132" s="2"/>
       <c r="B132" t="s">
         <v>79</v>
       </c>
-      <c r="C132" s="3"/>
+      <c r="C132" s="3" t="s">
+        <v>464</v>
+      </c>
     </row>
     <row r="133" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A133" s="2" t="s">
-        <v>440</v>
+        <v>435</v>
       </c>
       <c r="B133" t="s">
-        <v>439</v>
+        <v>434</v>
       </c>
       <c r="C133" s="3"/>
     </row>
@@ -4286,22 +4304,22 @@
     </row>
     <row r="138" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A138" s="20" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="C138" s="3"/>
     </row>
     <row r="139" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A139" s="4" t="s">
-        <v>441</v>
+        <v>436</v>
       </c>
       <c r="B139" s="21" t="s">
-        <v>442</v>
+        <v>437</v>
       </c>
       <c r="C139" s="5"/>
     </row>
     <row r="143" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A143" s="8" t="s">
-        <v>444</v>
+        <v>439</v>
       </c>
       <c r="B143" s="19"/>
       <c r="C143" s="19"/>
@@ -4312,164 +4330,108 @@
     </row>
     <row r="144" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A144" s="2"/>
-      <c r="B144" s="28" t="s">
+      <c r="B144" t="s">
         <v>79</v>
       </c>
-      <c r="C144" s="28"/>
-      <c r="D144" s="28"/>
-      <c r="E144" s="28"/>
-      <c r="F144" s="28"/>
       <c r="G144" s="3"/>
     </row>
     <row r="145" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A145" s="2"/>
-      <c r="B145" s="28" t="s">
+      <c r="B145" t="s">
         <v>69</v>
       </c>
-      <c r="C145" s="28"/>
-      <c r="D145" s="28"/>
-      <c r="E145" s="28"/>
-      <c r="F145" s="28"/>
       <c r="G145" s="3"/>
     </row>
     <row r="146" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A146" s="2"/>
-      <c r="B146" s="28" t="s">
+      <c r="B146" t="s">
         <v>193</v>
       </c>
-      <c r="C146" s="28"/>
-      <c r="D146" s="28"/>
-      <c r="E146" s="28"/>
-      <c r="F146" s="28"/>
       <c r="G146" s="3"/>
     </row>
     <row r="147" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A147" s="2"/>
-      <c r="B147" s="28" t="s">
-        <v>451</v>
-      </c>
-      <c r="C147" s="28"/>
-      <c r="D147" s="28"/>
-      <c r="E147" s="28"/>
-      <c r="F147" s="28"/>
+      <c r="B147" t="s">
+        <v>446</v>
+      </c>
       <c r="G147" s="3"/>
     </row>
     <row r="148" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A148" s="2"/>
-      <c r="B148" s="28" t="s">
-        <v>445</v>
-      </c>
-      <c r="C148" s="28"/>
-      <c r="D148" s="28"/>
-      <c r="E148" s="28"/>
-      <c r="F148" s="28"/>
+      <c r="B148" t="s">
+        <v>440</v>
+      </c>
       <c r="G148" s="3"/>
     </row>
     <row r="149" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A149" s="2"/>
-      <c r="B149" s="28" t="s">
-        <v>446</v>
-      </c>
-      <c r="C149" s="28"/>
-      <c r="D149" s="28"/>
-      <c r="E149" s="28"/>
-      <c r="F149" s="28"/>
+      <c r="B149" t="s">
+        <v>441</v>
+      </c>
       <c r="G149" s="3"/>
     </row>
     <row r="150" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A150" s="2"/>
-      <c r="B150" s="28" t="s">
-        <v>450</v>
-      </c>
-      <c r="C150" s="28"/>
-      <c r="D150" s="28"/>
-      <c r="E150" s="28"/>
-      <c r="F150" s="28"/>
+      <c r="B150" t="s">
+        <v>445</v>
+      </c>
       <c r="G150" s="3"/>
     </row>
     <row r="151" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A151" s="2"/>
-      <c r="B151" s="28" t="s">
-        <v>449</v>
-      </c>
-      <c r="C151" s="28"/>
-      <c r="D151" s="28"/>
-      <c r="E151" s="28"/>
-      <c r="F151" s="28"/>
+      <c r="B151" t="s">
+        <v>444</v>
+      </c>
       <c r="G151" s="3"/>
     </row>
     <row r="152" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A152" s="2"/>
-      <c r="B152" s="28" t="s">
-        <v>439</v>
-      </c>
-      <c r="C152" s="28"/>
-      <c r="D152" s="28"/>
-      <c r="E152" s="28"/>
-      <c r="F152" s="28"/>
+      <c r="B152" t="s">
+        <v>434</v>
+      </c>
       <c r="G152" s="3"/>
     </row>
     <row r="153" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A153" s="2"/>
-      <c r="B153" s="28"/>
-      <c r="C153" s="28"/>
-      <c r="D153" s="28"/>
-      <c r="E153" s="28"/>
-      <c r="F153" s="28"/>
       <c r="G153" s="3"/>
     </row>
     <row r="154" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A154" s="20" t="s">
-        <v>389</v>
-      </c>
-      <c r="B154" s="28"/>
-      <c r="C154" s="28"/>
-      <c r="D154" s="28"/>
-      <c r="E154" s="28"/>
-      <c r="F154" s="28"/>
+        <v>387</v>
+      </c>
       <c r="G154" s="3"/>
     </row>
     <row r="155" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A155" s="2" t="s">
-        <v>447</v>
-      </c>
-      <c r="B155" s="28" t="s">
-        <v>448</v>
-      </c>
-      <c r="C155" s="28" t="s">
-        <v>457</v>
-      </c>
-      <c r="D155" s="28"/>
-      <c r="E155" s="28"/>
-      <c r="F155" s="28"/>
+        <v>442</v>
+      </c>
+      <c r="B155" t="s">
+        <v>443</v>
+      </c>
+      <c r="C155" t="s">
+        <v>452</v>
+      </c>
       <c r="G155" s="3"/>
     </row>
     <row r="156" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A156" s="2" t="s">
-        <v>452</v>
-      </c>
-      <c r="B156" s="28" t="s">
-        <v>453</v>
-      </c>
-      <c r="C156" s="28" t="s">
-        <v>454</v>
-      </c>
-      <c r="D156" s="28"/>
-      <c r="E156" s="28"/>
-      <c r="F156" s="28"/>
+        <v>447</v>
+      </c>
+      <c r="B156" t="s">
+        <v>448</v>
+      </c>
+      <c r="C156" t="s">
+        <v>449</v>
+      </c>
       <c r="G156" s="3"/>
     </row>
     <row r="157" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A157" s="2" t="s">
-        <v>455</v>
-      </c>
-      <c r="B157" s="28" t="s">
-        <v>456</v>
-      </c>
-      <c r="C157" s="28"/>
-      <c r="D157" s="28"/>
-      <c r="E157" s="28"/>
-      <c r="F157" s="28"/>
+        <v>450</v>
+      </c>
+      <c r="B157" t="s">
+        <v>451</v>
+      </c>
       <c r="G157" s="3"/>
     </row>
     <row r="158" spans="1:7" x14ac:dyDescent="0.35">
@@ -4483,28 +4445,28 @@
     </row>
     <row r="161" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A161" s="8" t="s">
-        <v>458</v>
+        <v>453</v>
       </c>
       <c r="B161" s="19"/>
       <c r="C161" s="9"/>
     </row>
     <row r="162" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A162" s="2"/>
-      <c r="B162" s="28" t="s">
+      <c r="B162" t="s">
         <v>79</v>
       </c>
       <c r="C162" s="3"/>
     </row>
     <row r="163" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A163" s="2"/>
-      <c r="B163" s="28" t="s">
+      <c r="B163" t="s">
         <v>69</v>
       </c>
       <c r="C163" s="3"/>
     </row>
     <row r="164" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A164" s="2"/>
-      <c r="B164" s="28" t="s">
+      <c r="B164" t="s">
         <v>146</v>
       </c>
       <c r="C164" s="3"/>
@@ -4513,64 +4475,60 @@
       <c r="A165" s="2" t="s">
         <v>143</v>
       </c>
-      <c r="B165" s="28" t="s">
-        <v>459</v>
+      <c r="B165" t="s">
+        <v>454</v>
       </c>
       <c r="C165" s="3"/>
     </row>
     <row r="166" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A166" s="2"/>
-      <c r="B166" s="28" t="s">
+      <c r="B166" t="s">
         <v>145</v>
       </c>
       <c r="C166" s="3"/>
     </row>
     <row r="167" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A167" s="2"/>
-      <c r="B167" s="28"/>
       <c r="C167" s="3"/>
     </row>
     <row r="168" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A168" s="2"/>
-      <c r="B168" s="28"/>
       <c r="C168" s="3"/>
     </row>
     <row r="169" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A169" s="2"/>
-      <c r="B169" s="28"/>
       <c r="C169" s="3"/>
     </row>
     <row r="170" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A170" s="20" t="s">
-        <v>389</v>
-      </c>
-      <c r="B170" s="28"/>
+        <v>387</v>
+      </c>
       <c r="C170" s="3"/>
     </row>
     <row r="171" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A171" s="2" t="s">
-        <v>460</v>
-      </c>
-      <c r="B171" s="28" t="s">
-        <v>461</v>
+        <v>455</v>
+      </c>
+      <c r="B171" t="s">
+        <v>456</v>
       </c>
       <c r="C171" s="3"/>
     </row>
     <row r="172" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A172" s="2" t="s">
-        <v>462</v>
-      </c>
-      <c r="B172" s="28" t="s">
-        <v>463</v>
+        <v>457</v>
+      </c>
+      <c r="B172" t="s">
+        <v>458</v>
       </c>
       <c r="C172" s="3"/>
     </row>
     <row r="173" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A173" s="2" t="s">
-        <v>464</v>
-      </c>
-      <c r="B173" s="28" t="s">
-        <v>465</v>
+        <v>459</v>
+      </c>
+      <c r="B173" t="s">
+        <v>460</v>
       </c>
       <c r="C173" s="3"/>
     </row>
@@ -5352,7 +5310,7 @@
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A104" s="2" t="s">
-        <v>437</v>
+        <v>432</v>
       </c>
       <c r="B104" s="3" t="s">
         <v>23</v>

</xml_diff>